<commit_message>
Added class diagram. Finalized the code and design of the application.
</commit_message>
<xml_diff>
--- a/SignatureApp/Rates/ErrorRates(Vladislav Galkov).xlsx
+++ b/SignatureApp/Rates/ErrorRates(Vladislav Galkov).xlsx
@@ -203,7 +203,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="0">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="3">
@@ -239,13 +239,13 @@
         <v>7</v>
       </c>
       <c r="B5" s="0">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C5" s="0">
         <v>0</v>
       </c>
       <c r="D5" s="0">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="6">
@@ -354,10 +354,10 @@
         <v>0</v>
       </c>
       <c r="C13" s="0">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -365,13 +365,13 @@
         <v>16</v>
       </c>
       <c r="B14" s="0">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="0">
         <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>0</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="15">
@@ -455,7 +455,7 @@
         <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -508,10 +508,10 @@
         <v>0.1</v>
       </c>
       <c r="C24" s="0">
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>0.15000000000000002</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="25">
@@ -575,13 +575,13 @@
         <v>31</v>
       </c>
       <c r="B29" s="0">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="C29" s="0">
         <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30">

</xml_diff>